<commit_message>
Aggiornamento dati e risultati
</commit_message>
<xml_diff>
--- a/dati/dati_ISS_età.xlsx
+++ b/dati/dati_ISS_età.xlsx
@@ -577,7 +577,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -15932,7 +15932,7 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
@@ -15994,7 +15994,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
@@ -16056,7 +16056,7 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -16118,7 +16118,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
@@ -16180,7 +16180,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="2">
-        <v>44699</v>
+        <v>44706</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>

</xml_diff>